<commit_message>
Subir Actas y Actualizacion de Bitacora
</commit_message>
<xml_diff>
--- a/BTACORA.xlsx
+++ b/BTACORA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProyectoFinalCarrera\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBD3272-94A5-438D-B7A6-DC1375BBCBCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95087EC-C24A-415B-9CCC-B3399F0BDA2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{7CF5FC7B-D953-4CCD-9A08-2438F9C02DCD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7CF5FC7B-D953-4CCD-9A08-2438F9C02DCD}"/>
   </bookViews>
   <sheets>
     <sheet name="REGISTRO" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>REUNION</t>
   </si>
@@ -71,12 +71,24 @@
   </si>
   <si>
     <t>CAPACITACION</t>
+  </si>
+  <si>
+    <t>SE SIGUE EN CONFECCION DE ANTEPROYECTO</t>
+  </si>
+  <si>
+    <t>ENTREVISTA CON SUBJEFE OPERATIVO SILVIA DELGADO</t>
+  </si>
+  <si>
+    <t>ENTREVISTA CON SUBJEFE OPERATIVO MARIEL FERREIRA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -123,9 +135,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,14 +452,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3E5CB64-B399-4691-A3EA-1EA8C208F2AC}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="11.5546875" style="3"/>
     <col min="2" max="2" width="17.77734375" customWidth="1"/>
     <col min="3" max="3" width="81.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.21875" bestFit="1" customWidth="1"/>
@@ -455,7 +468,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
+      <c r="A1" s="3">
         <v>44286</v>
       </c>
       <c r="B1" t="s">
@@ -467,15 +480,15 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E1" s="1">
         <v>0.72916666666666663</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F1" s="1">
         <v>0.75</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+      <c r="A2" s="3">
         <v>44293</v>
       </c>
       <c r="B2" t="s">
@@ -484,15 +497,15 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>0.54166666666666663</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>0.625</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+      <c r="A3" s="3">
         <v>44299</v>
       </c>
       <c r="B3" t="s">
@@ -504,15 +517,15 @@
       <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>0.54166666666666663</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+      <c r="A4" s="3">
         <v>44300</v>
       </c>
       <c r="B4" t="s">
@@ -521,15 +534,61 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>0.83333333333333337</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>44301</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>44302</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>44306</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.60416666666666663</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -537,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80E890B8-5D4B-4E65-A6D2-2AA8F6F1C402}">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -557,7 +616,7 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>